<commit_message>
App and Firmware Update
Android App GUI upgrade
modified Firmware to include verison numbers
</commit_message>
<xml_diff>
--- a/Timesheets/2019-03-17.xlsx
+++ b/Timesheets/2019-03-17.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdemolde\Documents\GitHub\Coleman-Nordic-Butterfly\Timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CEEA50-9EF0-48EA-BE03-9F18190A938A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352D837C-60A5-4505-B22E-C9CBFC159B68}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>HR Office Use Only:</t>
     <phoneticPr fontId="8" type="noConversion"/>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>I certify that this report represents a reasonable estimate of the actual effort expended</t>
-  </si>
-  <si>
-    <t>during the period reported.</t>
   </si>
   <si>
     <t>Date:</t>
@@ -759,7 +753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -980,6 +974,54 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -992,86 +1034,34 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1558,7 +1548,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1602,7 +1592,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1630,7 +1620,7 @@
   <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31:J31"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.75"/>
@@ -1646,49 +1636,49 @@
     <row r="1" spans="1:18" ht="9" customHeight="1"/>
     <row r="2" spans="1:18" ht="23.1" customHeight="1">
       <c r="A2" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="84" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
-      <c r="Q2" s="85"/>
-      <c r="R2" s="85"/>
+        <v>12</v>
+      </c>
+      <c r="B2" s="98" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="99"/>
+      <c r="D2" s="99"/>
+      <c r="E2" s="99"/>
+      <c r="F2" s="99"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="99"/>
+      <c r="I2" s="99"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="99"/>
+      <c r="L2" s="99"/>
+      <c r="M2" s="99"/>
+      <c r="N2" s="99"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="99"/>
     </row>
     <row r="3" spans="1:18" ht="12.95" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
+        <v>11</v>
+      </c>
+      <c r="B3" s="100"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
+      <c r="O3" s="80"/>
+      <c r="P3" s="80"/>
+      <c r="Q3" s="80"/>
+      <c r="R3" s="80"/>
     </row>
     <row r="4" spans="1:18" ht="0.95" hidden="1" customHeight="1">
       <c r="B4" s="8"/>
@@ -1729,33 +1719,33 @@
       <c r="R5" s="14"/>
     </row>
     <row r="6" spans="1:18" ht="20.100000000000001" customHeight="1">
-      <c r="B6" s="93" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="93"/>
+      <c r="B6" s="107" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="107"/>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="106"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="106"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="79" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="80"/>
-      <c r="R6" s="80"/>
+      <c r="M6" s="94" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="95"/>
+      <c r="O6" s="95"/>
+      <c r="P6" s="95"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="95"/>
     </row>
     <row r="7" spans="1:18" ht="20.100000000000001" customHeight="1">
-      <c r="B7" s="89" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="90"/>
+      <c r="B7" s="103" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="104"/>
       <c r="D7" s="24"/>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
@@ -1765,14 +1755,14 @@
       <c r="J7" s="13"/>
       <c r="K7" s="11"/>
       <c r="L7" s="11"/>
-      <c r="M7" s="95" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="96"/>
-      <c r="O7" s="96"/>
-      <c r="P7" s="96"/>
-      <c r="Q7" s="96"/>
-      <c r="R7" s="96"/>
+      <c r="M7" s="81" t="s">
+        <v>17</v>
+      </c>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82"/>
     </row>
     <row r="8" spans="1:18" ht="11.1" customHeight="1">
       <c r="B8" s="11"/>
@@ -1815,11 +1805,11 @@
       <c r="R9" s="31"/>
     </row>
     <row r="10" spans="1:18" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="B10" s="106" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="102" t="s">
-        <v>16</v>
+      <c r="B10" s="92" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="88" t="s">
+        <v>14</v>
       </c>
       <c r="D10" s="65" t="s">
         <v>2</v>
@@ -1866,8 +1856,8 @@
       <c r="R10" s="7"/>
     </row>
     <row r="11" spans="1:18" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="B11" s="107"/>
-      <c r="C11" s="103"/>
+      <c r="B11" s="93"/>
+      <c r="C11" s="89"/>
       <c r="D11" s="64">
         <v>42079</v>
       </c>
@@ -1915,11 +1905,11 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="33" customHeight="1">
-      <c r="B12" s="101" t="s">
-        <v>26</v>
+      <c r="B12" s="87" t="s">
+        <v>24</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="38">
@@ -1948,18 +1938,20 @@
       <c r="N12" s="38">
         <v>4</v>
       </c>
-      <c r="O12" s="38"/>
+      <c r="O12" s="38">
+        <v>4.25</v>
+      </c>
       <c r="P12" s="38"/>
       <c r="Q12" s="39"/>
       <c r="R12" s="55">
         <f t="shared" ref="R12:R21" si="0">SUM(D12:Q12)</f>
-        <v>19.25</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="33" customHeight="1" thickBot="1">
-      <c r="B13" s="98"/>
+      <c r="B13" s="84"/>
       <c r="C13" s="40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13" s="41"/>
       <c r="E13" s="42"/>
@@ -1981,9 +1973,9 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="33" customHeight="1">
-      <c r="B14" s="97"/>
+      <c r="B14" s="83"/>
       <c r="C14" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="46"/>
@@ -2005,9 +1997,9 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="33" customHeight="1" thickBot="1">
-      <c r="B15" s="98"/>
+      <c r="B15" s="84"/>
       <c r="C15" s="40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D15" s="41"/>
       <c r="E15" s="42"/>
@@ -2029,9 +2021,9 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="33" customHeight="1">
-      <c r="B16" s="97"/>
+      <c r="B16" s="83"/>
       <c r="C16" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="46"/>
@@ -2053,9 +2045,9 @@
       </c>
     </row>
     <row r="17" spans="2:18" ht="33" customHeight="1" thickBot="1">
-      <c r="B17" s="98"/>
+      <c r="B17" s="84"/>
       <c r="C17" s="40" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="41"/>
       <c r="E17" s="42"/>
@@ -2077,9 +2069,9 @@
       </c>
     </row>
     <row r="18" spans="2:18" ht="33" customHeight="1">
-      <c r="B18" s="97"/>
+      <c r="B18" s="83"/>
       <c r="C18" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="46"/>
@@ -2101,9 +2093,9 @@
       </c>
     </row>
     <row r="19" spans="2:18" ht="33" customHeight="1" thickBot="1">
-      <c r="B19" s="98"/>
+      <c r="B19" s="84"/>
       <c r="C19" s="40" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D19" s="41"/>
       <c r="E19" s="42"/>
@@ -2125,9 +2117,9 @@
       </c>
     </row>
     <row r="20" spans="2:18" ht="33" customHeight="1">
-      <c r="B20" s="104"/>
+      <c r="B20" s="90"/>
       <c r="C20" s="44" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D20" s="45"/>
       <c r="E20" s="46"/>
@@ -2149,9 +2141,9 @@
       </c>
     </row>
     <row r="21" spans="2:18" ht="33" customHeight="1" thickBot="1">
-      <c r="B21" s="105"/>
+      <c r="B21" s="91"/>
       <c r="C21" s="48" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21" s="49"/>
       <c r="E21" s="46"/>
@@ -2173,10 +2165,10 @@
       </c>
     </row>
     <row r="22" spans="2:18" ht="35.1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B22" s="87" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="88"/>
+      <c r="B22" s="101" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="102"/>
       <c r="D22" s="59">
         <f t="shared" ref="D22:Q22" si="1">SUM(D12:D21)</f>
         <v>0</v>
@@ -2223,7 +2215,7 @@
       </c>
       <c r="O22" s="69">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="P22" s="69">
         <f t="shared" si="1"/>
@@ -2235,15 +2227,15 @@
       </c>
       <c r="R22" s="58">
         <f>SUM(D22:Q22)</f>
-        <v>19.25</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="29.1" customHeight="1">
       <c r="E23" s="51" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F23" s="78" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="R23" s="3"/>
     </row>
@@ -2252,7 +2244,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -2266,7 +2258,7 @@
     </row>
     <row r="25" spans="2:18" ht="15.95" customHeight="1">
       <c r="B25" s="51" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C25" s="20"/>
       <c r="D25"/>
@@ -2274,8 +2266,8 @@
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25"/>
-      <c r="I25" s="81"/>
-      <c r="J25" s="82"/>
+      <c r="I25" s="96"/>
+      <c r="J25" s="97"/>
       <c r="K25" s="70"/>
       <c r="L25" s="71"/>
       <c r="M25" s="71"/>
@@ -2289,8 +2281,8 @@
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="H26"/>
-      <c r="I26" s="99"/>
-      <c r="J26" s="100"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="86"/>
       <c r="K26" s="75"/>
       <c r="L26" s="75"/>
       <c r="M26" s="75"/>
@@ -2305,12 +2297,12 @@
       <c r="C27" s="34"/>
       <c r="D27" s="6"/>
       <c r="E27" s="52" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="15"/>
-      <c r="I27" s="83"/>
-      <c r="J27" s="83"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="80"/>
       <c r="K27" s="75"/>
       <c r="L27" s="75"/>
       <c r="M27" s="75"/>
@@ -2322,15 +2314,15 @@
     </row>
     <row r="28" spans="2:18" ht="17.100000000000001" customHeight="1" thickBot="1">
       <c r="B28" s="53" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
       <c r="F28" s="23"/>
       <c r="G28" s="23"/>
-      <c r="I28" s="83"/>
-      <c r="J28" s="83"/>
+      <c r="I28" s="80"/>
+      <c r="J28" s="80"/>
       <c r="K28" s="75"/>
       <c r="L28" s="75"/>
       <c r="M28" s="75"/>
@@ -2342,16 +2334,16 @@
     </row>
     <row r="29" spans="2:18" ht="21.95" customHeight="1" thickTop="1">
       <c r="B29" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="H29" s="108"/>
-      <c r="I29" s="109"/>
-      <c r="J29" s="109"/>
+      <c r="H29"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="80"/>
       <c r="K29" s="75"/>
       <c r="L29" s="75"/>
       <c r="M29" s="75"/>
@@ -2363,16 +2355,16 @@
     </row>
     <row r="30" spans="2:18" ht="21.95" customHeight="1">
       <c r="B30" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
-      <c r="H30" s="108"/>
-      <c r="I30" s="83"/>
-      <c r="J30" s="83"/>
+      <c r="H30"/>
+      <c r="I30" s="80"/>
+      <c r="J30" s="80"/>
       <c r="K30" s="75"/>
       <c r="L30" s="75"/>
       <c r="M30" s="75"/>
@@ -2385,8 +2377,8 @@
     <row r="31" spans="2:18" ht="21.95" customHeight="1">
       <c r="D31"/>
       <c r="G31"/>
-      <c r="I31" s="94"/>
-      <c r="J31" s="94"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="79"/>
     </row>
     <row r="32" spans="2:18" ht="21.95" customHeight="1">
       <c r="B32"/>
@@ -2419,6 +2411,15 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="M6:R6"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="B2:R2"/>
+    <mergeCell ref="B3:R3"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="I31:J31"/>
     <mergeCell ref="I30:J30"/>
     <mergeCell ref="M7:R7"/>
@@ -2432,15 +2433,6 @@
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="M6:R6"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="B2:R2"/>
-    <mergeCell ref="B3:R3"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="B6:C6"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>